<commit_message>
upgarde to new masterlist
</commit_message>
<xml_diff>
--- a/storage/app/Colombo_re_upload.xlsx
+++ b/storage/app/Colombo_re_upload.xlsx
@@ -677,7 +677,9 @@
       <c r="C6">
         <v>7</v>
       </c>
-      <c r="D6"/>
+      <c r="D6">
+        <v>8</v>
+      </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
@@ -707,7 +709,9 @@
       <c r="C7">
         <v>8</v>
       </c>
-      <c r="D7"/>
+      <c r="D7">
+        <v>9</v>
+      </c>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>

</xml_diff>